<commit_message>
bar is no more
</commit_message>
<xml_diff>
--- a/ProgettoDB/res/tables/MaleniaData.xlsx
+++ b/ProgettoDB/res/tables/MaleniaData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Progetto\Hotel-Malenia\res\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Progetto\Hotel-Malenia\ProgettoDB\res\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16698A8-921F-4F38-B6A7-E56475C8F550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D771564-1B29-4DCE-BE0D-AD65051241D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{1E9E1B00-858F-4184-A9F3-6F302A51F4E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1E9E1B00-858F-4184-A9F3-6F302A51F4E6}"/>
   </bookViews>
   <sheets>
     <sheet name="prezziHotel" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="162">
   <si>
     <t>Concetto</t>
   </si>
@@ -591,12 +591,6 @@
   </si>
   <si>
     <t>Piano tariffario dell'hotel che garantisce al cliente la permanenza nella struttura, la consumazione gratuita dei 3 pasti principali della giornata e una base di servizi che normalmente sarebbero a pagamento.</t>
-  </si>
-  <si>
-    <t>Richiesta specifica di una bevanda a base di caffè che non è prevista nel menù.</t>
-  </si>
-  <si>
-    <t>Consumazione extra</t>
   </si>
   <si>
     <t>Volume</t>
@@ -1130,7 +1124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1258,15 +1252,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1312,7 +1297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1391,21 +1376,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -2057,8 +2036,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5091C1EE-B360-4EEE-AF61-8F7CBC61D816}" name="Tabella17" displayName="Tabella17" ref="D4:F16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
-  <autoFilter ref="D4:F16" xr:uid="{5091C1EE-B360-4EEE-AF61-8F7CBC61D816}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5091C1EE-B360-4EEE-AF61-8F7CBC61D816}" name="Tabella17" displayName="Tabella17" ref="D4:F15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
+  <autoFilter ref="D4:F15" xr:uid="{5091C1EE-B360-4EEE-AF61-8F7CBC61D816}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CE1965F7-5B83-469B-BAE1-B40A3E6BABF7}" name="TERMINE" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{4F3175D3-AC56-4BA9-8783-0AE12AF49FAA}" name="BREVE DESCRIZIONE" dataDxfId="1"/>
@@ -2786,22 +2765,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="5">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75EF582-CC88-40FD-A68C-9579BA74413F}">
-  <dimension ref="D3:O16"/>
+  <dimension ref="D3:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,21 +2916,11 @@
       </c>
       <c r="F15" s="35"/>
     </row>
-    <row r="16" spans="4:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="D16" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>117</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2975,273 +2945,274 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>118</v>
+      <c r="B5" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="40">
+      <c r="B6" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="38">
         <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="42">
+      <c r="B7" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="40">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="42">
+      <c r="A8" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="40">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="42">
+      <c r="B11" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="40">
         <v>10000</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="42">
+      <c r="B12" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="40">
         <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="42">
+      <c r="B13" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="40">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="42">
+      <c r="B14" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="40">
         <v>1000000</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="42">
+      <c r="B17" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="40">
         <v>1000</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="42">
+      <c r="A18" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="40">
         <v>100000</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="42">
+      <c r="B19" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="40">
         <v>10000</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="42">
+      <c r="B22" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="40">
         <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="42">
+      <c r="B23" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="40">
         <v>100000</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="42">
+      <c r="A24" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="40">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="44">
+      <c r="A27" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="42">
         <v>3000</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="42">
+      <c r="A28" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="40">
         <v>3000</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="41">
+      <c r="B29" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="39">
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="42">
+      <c r="A32" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="40">
         <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="B33" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="46">
+      <c r="A33" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="44">
         <v>1</v>
       </c>
       <c r="E33" s="3"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="42">
+      <c r="B36" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="42">
+      <c r="B37" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="40">
         <v>10000</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="42">
+      <c r="B38" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="40">
         <v>10000</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="42">
+      <c r="A39" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="40">
         <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3260,14 +3231,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>127</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3275,10 +3246,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3286,10 +3257,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3297,10 +3268,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3308,10 +3279,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3319,10 +3290,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3330,10 +3301,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3341,10 +3312,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3352,10 +3323,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3363,10 +3334,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3374,10 +3345,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3385,10 +3356,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3396,14 +3367,15 @@
         <v>12</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3921,7 +3893,7 @@
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
       <c r="D42" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E42" s="17"/>
     </row>
@@ -4749,7 +4721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5EC3296-8FDF-4C89-A16A-D342517C31E8}">
   <dimension ref="B1:E133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A115" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -4897,8 +4869,8 @@
         <v>32</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="48" t="s">
-        <v>155</v>
+      <c r="D13" s="46" t="s">
+        <v>153</v>
       </c>
       <c r="E13" s="7"/>
     </row>
@@ -5004,7 +4976,7 @@
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E21" s="17"/>
     </row>
@@ -5140,11 +5112,11 @@
     <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="D34" s="48" t="s">
-        <v>155</v>
+      <c r="D34" s="46" t="s">
+        <v>153</v>
       </c>
       <c r="E34" s="7"/>
     </row>
@@ -5278,18 +5250,18 @@
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
       <c r="D44" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E44" s="17"/>
     </row>
     <row r="51" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C52" s="6"/>
-      <c r="D52" s="48" t="s">
-        <v>155</v>
+      <c r="D52" s="46" t="s">
+        <v>153</v>
       </c>
       <c r="E52" s="7"/>
     </row>
@@ -5409,7 +5381,7 @@
       <c r="B61" s="14"/>
       <c r="C61" s="15"/>
       <c r="D61" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E61" s="17"/>
     </row>
@@ -5545,11 +5517,11 @@
     <row r="73" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C74" s="6"/>
-      <c r="D74" s="48" t="s">
-        <v>155</v>
+      <c r="D74" s="46" t="s">
+        <v>153</v>
       </c>
       <c r="E74" s="7"/>
     </row>
@@ -5655,18 +5627,18 @@
       <c r="B82" s="14"/>
       <c r="C82" s="15"/>
       <c r="D82" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E82" s="17"/>
     </row>
     <row r="83" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="46" t="s">
         <v>153</v>
-      </c>
-      <c r="C84" s="6"/>
-      <c r="D84" s="48" t="s">
-        <v>155</v>
       </c>
       <c r="E84" s="7"/>
     </row>
@@ -6040,11 +6012,11 @@
     <row r="124" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C125" s="6"/>
-      <c r="D125" s="48" t="s">
-        <v>155</v>
+      <c r="D125" s="46" t="s">
+        <v>153</v>
       </c>
       <c r="E125" s="7"/>
     </row>
@@ -6150,7 +6122,7 @@
       <c r="B133" s="14"/>
       <c r="C133" s="15"/>
       <c r="D133" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E133" s="17"/>
     </row>

</xml_diff>

<commit_message>
adapting new context to review and fixing projects logic problems
</commit_message>
<xml_diff>
--- a/ProgettoDB/res/tables/MaleniaData.xlsx
+++ b/ProgettoDB/res/tables/MaleniaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Progetto\Hotel-Malenia\ProgettoDB\res\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Hotel-Malenia\ProgettoDB\res\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D771564-1B29-4DCE-BE0D-AD65051241D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBB0E3E-8B31-405E-AC2E-A7B5DF340F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1E9E1B00-858F-4184-A9F3-6F302A51F4E6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1E9E1B00-858F-4184-A9F3-6F302A51F4E6}"/>
   </bookViews>
   <sheets>
     <sheet name="prezziHotel" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="145">
   <si>
     <t>Concetto</t>
   </si>
@@ -407,85 +407,19 @@
     <t>COSTO GIORNALIERO - FAMILIARE</t>
   </si>
   <si>
-    <t>PRODOTTO</t>
-  </si>
-  <si>
-    <t>LISTINO ALL - INCLUSIVE</t>
-  </si>
-  <si>
-    <t>LISTINO NORMALE</t>
-  </si>
-  <si>
-    <t>Caffè</t>
-  </si>
-  <si>
-    <t>Gratuito</t>
-  </si>
-  <si>
-    <t>Cappuccino</t>
-  </si>
-  <si>
     <t>SERVIZI HOTEL</t>
   </si>
   <si>
-    <t>Infuso</t>
-  </si>
-  <si>
     <t>Lettino Spiaggia</t>
   </si>
   <si>
-    <t>Già compresa nel pacchetto</t>
-  </si>
-  <si>
-    <t>Variante caffetteria</t>
-  </si>
-  <si>
     <t>Palestra</t>
   </si>
   <si>
-    <t>Spremuta</t>
-  </si>
-  <si>
     <t>Casinò</t>
   </si>
   <si>
-    <t>Succo</t>
-  </si>
-  <si>
     <t>Parcheggio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bevanda </t>
-  </si>
-  <si>
-    <t>Colazione in camera</t>
-  </si>
-  <si>
-    <t>10,00 € a persona</t>
-  </si>
-  <si>
-    <t>Calice vino</t>
-  </si>
-  <si>
-    <t>Variabile</t>
-  </si>
-  <si>
-    <t>Bottiglia vino</t>
-  </si>
-  <si>
-    <t>Birra media</t>
-  </si>
-  <si>
-    <t>Birra grande</t>
-  </si>
-  <si>
-    <t>Spritz</t>
-  </si>
-  <si>
-    <t>Analcolico</t>
-  </si>
-  <si>
-    <t>Cocktail</t>
   </si>
   <si>
     <t>SERVIZI BENESSERE</t>
@@ -522,9 +456,6 @@
     <t>Turista</t>
   </si>
   <si>
-    <t>Oggetto che riporta i dati personali di un cliente.</t>
-  </si>
-  <si>
     <t>Membro del personale</t>
   </si>
   <si>
@@ -543,25 +474,10 @@
     <t>Mansione</t>
   </si>
   <si>
-    <t>Listino</t>
-  </si>
-  <si>
-    <t>Quantità di denaro necessaria per poter ottenere una eventuale prestazione oppure per poter acquasitare una bevanda o un prodotto.</t>
-  </si>
-  <si>
-    <t>Prezzo, Costo</t>
-  </si>
-  <si>
     <t>Resoconto di pagamento</t>
   </si>
   <si>
-    <t>Quantità di denaro rimanente che il cliente deve versare all'hotel al termine del suo soggiorno.</t>
-  </si>
-  <si>
     <t>Permanenza temporanea in un luogo.</t>
-  </si>
-  <si>
-    <t>Villeggiatura</t>
   </si>
   <si>
     <t>Servizio</t>
@@ -578,16 +494,6 @@
   </si>
   <si>
     <t>Stanza della struttura in grado di accogliere un nucleo familiare di 4 oppure 5 persone.</t>
-  </si>
-  <si>
-    <t>Pensiona completa</t>
-  </si>
-  <si>
-    <t>Piano tariffario dell'hotel che garantisce al
-cliente la permanenza nella struttura e la consumazione gratuita dei 3 pasti principali della giornata.</t>
-  </si>
-  <si>
-    <t>All-inclusive</t>
   </si>
   <si>
     <t>Piano tariffario dell'hotel che garantisce al cliente la permanenza nella struttura, la consumazione gratuita dei 3 pasti principali della giornata e una base di servizi che normalmente sarebbero a pagamento.</t>
@@ -1049,6 +955,48 @@
   </si>
   <si>
     <t>OP 12 - Generazione documento</t>
+  </si>
+  <si>
+    <t>Oggetto che riporta i dati personali e il resoconto di un cliente.</t>
+  </si>
+  <si>
+    <t>Quantità di denaro necessaria per poter usufruire di un eventuale servizio.</t>
+  </si>
+  <si>
+    <t>Quantità di denaro rappresentante il debito del cliente nei confronti dell'hotel.</t>
+  </si>
+  <si>
+    <t>Villeggiatura, Vacanza</t>
+  </si>
+  <si>
+    <t>Piano tariffario dell'hotel che garantisce al cliente la permanenza nella struttura e la consumazione gratuita dei 3 pasti principali della giornata.</t>
+  </si>
+  <si>
+    <t>Bed&amp;Breakfast (BB)</t>
+  </si>
+  <si>
+    <t>Piano tariffario</t>
+  </si>
+  <si>
+    <t>Costo</t>
+  </si>
+  <si>
+    <t>Prezzo, Tariffa</t>
+  </si>
+  <si>
+    <t>Piano tariffario dell'hotel che garantisce la permanenza nella struttura e la colazione della mattina seguente, questo fino al termine del periodo di soggiorno.</t>
+  </si>
+  <si>
+    <t>Offerta data ai clienti per poter usufruire, secondo varie possibilità, dei servizi offerti dall'hotel. Il piano tariffario varia e di conseguenza ne varia anche il suo costo.</t>
+  </si>
+  <si>
+    <t>Pacchetto vacanza.</t>
+  </si>
+  <si>
+    <t>Pensiona completa (PC)</t>
+  </si>
+  <si>
+    <t>All-inclusive (ALI)</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1046,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1108,12 +1056,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1297,7 +1239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1349,18 +1291,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1376,7 +1306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -1385,13 +1315,37 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1593,6 +1547,64 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1608,6 +1620,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1695,6 +1723,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1755,212 +1799,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1975,73 +1813,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B81FD6EF-9C3F-4B92-BE77-80A5DB308398}" name="Tabella1" displayName="Tabella1" ref="D4:G7" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
-  <autoFilter ref="D4:G7" xr:uid="{B81FD6EF-9C3F-4B92-BE77-80A5DB308398}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B81FD6EF-9C3F-4B92-BE77-80A5DB308398}" name="Tabella1" displayName="Tabella1" ref="B4:E7" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
+  <autoFilter ref="B4:E7" xr:uid="{B81FD6EF-9C3F-4B92-BE77-80A5DB308398}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EDB5CAB9-859E-4CA5-BC74-2C52F6836EE4}" name="PACCHETTO VACANZE" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{0569EA2E-A953-44E4-92B1-5381D27F006F}" name="COSTO SETTIMANALE - SINGOLA" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{23F2F3A9-F159-4A53-8D52-8710B82F343C}" name="COSTO SETTIMANALE - DOPPIA" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{63AFC297-D316-4925-9353-CAFCB5941A96}" name="COSTO SETTIMANALE - FAMILIARE" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{EDB5CAB9-859E-4CA5-BC74-2C52F6836EE4}" name="PACCHETTO VACANZE" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{0569EA2E-A953-44E4-92B1-5381D27F006F}" name="COSTO SETTIMANALE - SINGOLA" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{23F2F3A9-F159-4A53-8D52-8710B82F343C}" name="COSTO SETTIMANALE - DOPPIA" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{63AFC297-D316-4925-9353-CAFCB5941A96}" name="COSTO SETTIMANALE - FAMILIARE" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81903738-74C5-4093-9441-E414A4DD48D1}" name="Tabella13" displayName="Tabella13" ref="D9:G12" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
-  <autoFilter ref="D9:G12" xr:uid="{81903738-74C5-4093-9441-E414A4DD48D1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81903738-74C5-4093-9441-E414A4DD48D1}" name="Tabella13" displayName="Tabella13" ref="B9:E12" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="B9:E12" xr:uid="{81903738-74C5-4093-9441-E414A4DD48D1}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A8ED6124-E717-48ED-9F89-5149D3AB29C1}" name="PACCHETTO VACANZE" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{F98C636A-37DE-4DBC-B03F-984EBA52ACE2}" name="COSTO GIORNALIERO - SINGOLA" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{E37DD224-ACBC-4487-881B-4C74A17BD987}" name="COSTO GIORNALIERO - DOPPIA" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{A9F0470A-4902-48E2-8CD3-25A516BEC109}" name="COSTO GIORNALIERO - FAMILIARE" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{A8ED6124-E717-48ED-9F89-5149D3AB29C1}" name="PACCHETTO VACANZE" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{F98C636A-37DE-4DBC-B03F-984EBA52ACE2}" name="COSTO GIORNALIERO - SINGOLA" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{E37DD224-ACBC-4487-881B-4C74A17BD987}" name="COSTO GIORNALIERO - DOPPIA" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{A9F0470A-4902-48E2-8CD3-25A516BEC109}" name="COSTO GIORNALIERO - FAMILIARE" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4CCD44E5-2463-400A-84AD-2A6CD64F78C6}" name="Tabella3" displayName="Tabella3" ref="E14:G31" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="E14:G31" xr:uid="{4CCD44E5-2463-400A-84AD-2A6CD64F78C6}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4AFFAFFF-BEE3-4EFD-8B6B-5229A5A4B4E8}" name="PRODOTTO" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{E679302A-196A-4009-96E9-6A6F1CB5152B}" name="LISTINO ALL - INCLUSIVE" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{C21D109A-4208-4EB4-B17D-34E9D1775E96}" name="LISTINO NORMALE" dataDxfId="18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{941C4DBF-D34A-46B4-B864-22D8371CC577}" name="Tabella5" displayName="Tabella5" ref="B16:C20" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="B16:C20" xr:uid="{941C4DBF-D34A-46B4-B864-22D8371CC577}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FB130275-AA60-41A0-AB71-CF3DBCC02329}" name="SERVIZI BENESSERE" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{CF2B0D29-9BA0-45A3-9068-17D76570C828}" name="TARIFFE" dataDxfId="8"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7F890F25-0280-4E3A-8749-08A52ED362D7}" name="Tabella4" displayName="Tabella4" ref="I16:K20" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="I16:K20" xr:uid="{7F890F25-0280-4E3A-8749-08A52ED362D7}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A750A1CF-F4B8-4682-A3AD-89400730DD5C}" name="SERVIZI HOTEL" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{6D158294-0281-4EF0-A49E-C2BBC33D47C5}" name="LISTINO ALL - INCLUSIVE" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{766766E5-5D57-4AB0-91E0-8A762034663E}" name="LISTINO NORMALE" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7F890F25-0280-4E3A-8749-08A52ED362D7}" name="Tabella4" displayName="Tabella4" ref="B24:C28" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="B24:C28" xr:uid="{7F890F25-0280-4E3A-8749-08A52ED362D7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A750A1CF-F4B8-4682-A3AD-89400730DD5C}" name="SERVIZI HOTEL" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{6D158294-0281-4EF0-A49E-C2BBC33D47C5}" name="TARIFFE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{941C4DBF-D34A-46B4-B864-22D8371CC577}" name="Tabella5" displayName="Tabella5" ref="E34:F38" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="E34:F38" xr:uid="{941C4DBF-D34A-46B4-B864-22D8371CC577}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FB130275-AA60-41A0-AB71-CF3DBCC02329}" name="SERVIZI BENESSERE" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{CF2B0D29-9BA0-45A3-9068-17D76570C828}" name="TARIFFE" dataDxfId="7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5091C1EE-B360-4EEE-AF61-8F7CBC61D816}" name="Tabella17" displayName="Tabella17" ref="D4:F15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
-  <autoFilter ref="D4:F15" xr:uid="{5091C1EE-B360-4EEE-AF61-8F7CBC61D816}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5091C1EE-B360-4EEE-AF61-8F7CBC61D816}" name="Tabella17" displayName="Tabella17" ref="B1:D14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="B1:D14" xr:uid="{5091C1EE-B360-4EEE-AF61-8F7CBC61D816}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CE1965F7-5B83-469B-BAE1-B40A3E6BABF7}" name="TERMINE" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{4F3175D3-AC56-4BA9-8783-0AE12AF49FAA}" name="BREVE DESCRIZIONE" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{E69F55AF-1F81-4B44-9386-8AD677F0DB13}" name="SINONIMI" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CE1965F7-5B83-469B-BAE1-B40A3E6BABF7}" name="TERMINE" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4F3175D3-AC56-4BA9-8783-0AE12AF49FAA}" name="BREVE DESCRIZIONE" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E69F55AF-1F81-4B44-9386-8AD677F0DB13}" name="SINONIMI" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2344,581 +2169,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEFCC1C6-B524-482C-BB0D-810C064B0A12}">
-  <dimension ref="D4:K42"/>
+  <dimension ref="B4:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="24"/>
-    <col min="4" max="4" width="26.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="24"/>
-    <col min="13" max="13" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" style="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="3.42578125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="33.28515625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="24"/>
+    <col min="11" max="11" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="24" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="C4" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="D4" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="E4" s="45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="24" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
         <v>49</v>
       </c>
+      <c r="C5" s="25">
+        <v>400</v>
+      </c>
+      <c r="D5" s="25">
+        <v>650</v>
+      </c>
       <c r="E5" s="25">
-        <v>400</v>
-      </c>
-      <c r="F5" s="25">
-        <v>650</v>
-      </c>
-      <c r="G5" s="25">
         <v>1200</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D6" s="24" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
         <v>50</v>
       </c>
+      <c r="C6" s="25">
+        <v>500</v>
+      </c>
+      <c r="D6" s="25">
+        <v>900</v>
+      </c>
       <c r="E6" s="25">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="25">
+        <v>900</v>
+      </c>
+      <c r="D7" s="25">
+        <v>1700</v>
+      </c>
+      <c r="E7" s="25">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="25">
+        <v>60</v>
+      </c>
+      <c r="D10" s="25">
+        <v>100</v>
+      </c>
+      <c r="E10" s="25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="25">
+        <v>90</v>
+      </c>
+      <c r="D11" s="25">
+        <v>160</v>
+      </c>
+      <c r="E11" s="25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="25">
+        <v>150</v>
+      </c>
+      <c r="D12" s="25">
+        <v>280</v>
+      </c>
+      <c r="E12" s="25">
         <v>500</v>
       </c>
-      <c r="F6" s="25">
-        <v>900</v>
-      </c>
-      <c r="G6" s="25">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D7" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="25">
-        <v>900</v>
-      </c>
-      <c r="F7" s="25">
-        <v>1700</v>
-      </c>
-      <c r="G7" s="25">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D9" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="25">
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="26"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="25">
-        <v>100</v>
-      </c>
-      <c r="G10" s="25">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D11" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="25">
-        <v>90</v>
-      </c>
-      <c r="F11" s="25">
-        <v>160</v>
-      </c>
-      <c r="G11" s="25">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D12" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="25">
-        <v>150</v>
-      </c>
-      <c r="F12" s="25">
-        <v>280</v>
-      </c>
-      <c r="G12" s="25">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E14" s="24" t="s">
+      <c r="C16" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="26"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="C24" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="C25" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="24" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="24" t="s">
+      <c r="C26" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="C27" s="25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="26"/>
-      <c r="E16" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="25">
-        <v>1.4</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E17" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="25">
-        <v>2</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="25">
+      <c r="C28" s="25">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E18" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="25">
-        <v>3</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="K18" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="25">
-        <v>3.5</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="25">
-        <v>5</v>
-      </c>
-      <c r="K19" s="25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="25">
-        <v>3</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="J20" s="25">
-        <v>8</v>
-      </c>
-      <c r="K20" s="25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="27"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="29"/>
-    </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" s="26"/>
-    </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" s="30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="25">
-        <v>5</v>
-      </c>
-      <c r="G26" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="F27" s="25">
-        <v>7.5</v>
-      </c>
-      <c r="G27" s="25">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="28" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" s="25">
-        <v>8</v>
-      </c>
-      <c r="G29" s="25">
-        <v>8</v>
-      </c>
-      <c r="H29" s="26"/>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E30" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="25">
-        <v>6</v>
-      </c>
-      <c r="G30" s="25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E31" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="25">
-        <v>9</v>
-      </c>
-      <c r="G31" s="25">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E35" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F35" s="25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E36" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F36" s="25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E37" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F37" s="25">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E38" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F38" s="25">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="G40" s="26"/>
-    </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="H42" s="26"/>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="26"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="5">
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
-    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75EF582-CC88-40FD-A68C-9579BA74413F}">
-  <dimension ref="D3:O15"/>
+  <dimension ref="B1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="4:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="D5" s="31" t="s">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="4:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="D6" s="33" t="s">
+      <c r="C2" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="33"/>
-    </row>
-    <row r="7" spans="4:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="D7" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="4:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="D8" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="4:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="D9" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="4:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="D10" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="33"/>
-    </row>
-    <row r="11" spans="4:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="33" t="s">
+      <c r="C3" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="29"/>
+    </row>
+    <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="4:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="D12" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="4:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="D13" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="35"/>
-    </row>
-    <row r="14" spans="4:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="D14" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="F14" s="35"/>
-    </row>
-    <row r="15" spans="4:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="D15" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" s="35"/>
+      <c r="C8" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="31"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="44"/>
+    </row>
+    <row r="13" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="31"/>
+    </row>
+    <row r="14" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -2929,7 +2581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEDC950-AA2F-4131-8934-AB2918395EB7}">
   <dimension ref="A5:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2945,267 +2597,267 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>116</v>
+      <c r="B5" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="38">
+      <c r="B6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="34">
         <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="40">
+      <c r="B7" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="36">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="40">
+      <c r="A8" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="36">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="40">
+      <c r="B11" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="36">
         <v>10000</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="40">
+      <c r="B12" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="36">
         <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="40">
+      <c r="B13" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="36">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="40">
+      <c r="B14" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="36">
         <v>1000000</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="40">
+      <c r="B17" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="36">
         <v>1000</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="40">
+      <c r="A18" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="36">
         <v>100000</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="40">
+      <c r="B19" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="36">
         <v>10000</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="40">
+      <c r="B22" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="36">
         <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="40">
+      <c r="B23" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="36">
         <v>100000</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="40">
+      <c r="A24" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="36">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="42">
+      <c r="A27" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="38">
         <v>3000</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="40">
+      <c r="A28" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="36">
         <v>3000</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="39">
+      <c r="A29" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="35">
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="40">
+      <c r="A32" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="36">
         <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="44">
+      <c r="A33" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="40">
         <v>1</v>
       </c>
       <c r="E33" s="3"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="40">
+      <c r="B36" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="40">
+      <c r="B37" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="36">
         <v>10000</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="40">
+      <c r="B38" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="36">
         <v>10000</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B39" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="40">
+      <c r="A39" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="36">
         <v>100</v>
       </c>
     </row>
@@ -3231,14 +2883,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>127</v>
+      <c r="B4" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3246,10 +2898,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3257,10 +2909,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3268,10 +2920,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3279,10 +2931,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3290,10 +2942,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3301,10 +2953,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3312,10 +2964,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3323,10 +2975,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3334,10 +2986,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3345,10 +2997,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3356,10 +3008,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3367,10 +3019,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3893,7 +3545,7 @@
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
       <c r="D42" s="16" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="E42" s="17"/>
     </row>
@@ -4869,8 +4521,8 @@
         <v>32</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="46" t="s">
-        <v>153</v>
+      <c r="D13" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="E13" s="7"/>
     </row>
@@ -4976,7 +4628,7 @@
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="E21" s="17"/>
     </row>
@@ -5112,11 +4764,11 @@
     <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="D34" s="46" t="s">
-        <v>153</v>
+      <c r="D34" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="E34" s="7"/>
     </row>
@@ -5250,18 +4902,18 @@
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
       <c r="D44" s="16" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="E44" s="17"/>
     </row>
     <row r="51" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="C52" s="6"/>
-      <c r="D52" s="46" t="s">
-        <v>153</v>
+      <c r="D52" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="E52" s="7"/>
     </row>
@@ -5381,7 +5033,7 @@
       <c r="B61" s="14"/>
       <c r="C61" s="15"/>
       <c r="D61" s="16" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="E61" s="17"/>
     </row>
@@ -5517,11 +5169,11 @@
     <row r="73" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="C74" s="6"/>
-      <c r="D74" s="46" t="s">
-        <v>153</v>
+      <c r="D74" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="E74" s="7"/>
     </row>
@@ -5627,18 +5279,18 @@
       <c r="B82" s="14"/>
       <c r="C82" s="15"/>
       <c r="D82" s="16" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="E82" s="17"/>
     </row>
     <row r="83" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="C84" s="6"/>
-      <c r="D84" s="46" t="s">
-        <v>153</v>
+      <c r="D84" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="E84" s="7"/>
     </row>
@@ -6012,11 +5664,11 @@
     <row r="124" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="5" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="C125" s="6"/>
-      <c r="D125" s="46" t="s">
-        <v>153</v>
+      <c r="D125" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="E125" s="7"/>
     </row>
@@ -6122,7 +5774,7 @@
       <c r="B133" s="14"/>
       <c r="C133" s="15"/>
       <c r="D133" s="16" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="E133" s="17"/>
     </row>

</xml_diff>